<commit_message>
Check for null instead of String.Empty when reading multiple cells
</commit_message>
<xml_diff>
--- a/tests/MyExcel.UnitTests/MyExcel.xlsx
+++ b/tests/MyExcel.UnitTests/MyExcel.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26327"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27126"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\HP\source\repos\myexcel\lib\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\HP\source\repos\myexcel\tests\MyExcel.UnitTests\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A84D6D81-9968-437B-8E87-6620B284928E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{75547741-1E17-4412-A3F9-89DA6AFFF05F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3180" yWindow="0" windowWidth="17280" windowHeight="8880" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Plan1" sheetId="1" r:id="rId1"/>
@@ -25,9 +25,21 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1" uniqueCount="1">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="5">
   <si>
     <t>My Excel</t>
+  </si>
+  <si>
+    <t>created</t>
+  </si>
+  <si>
+    <t>was</t>
+  </si>
+  <si>
+    <t>with</t>
+  </si>
+  <si>
+    <t>love</t>
   </si>
 </sst>
 </file>
@@ -345,15 +357,49 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1"/>
+  <dimension ref="A1:E5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C1" sqref="C1"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
+        <v>4</v>
       </c>
     </row>
   </sheetData>

</xml_diff>